<commit_message>
Finished data collection, now working on the model
Former-commit-id: 611b9633b63ad6e1994f36317cd0734936b52b75 [formerly 8326e90952c762b8d2a13c3714dce0bd48692d73 [formerly 128a43666873d5192a089b0025318d5f21a758d6]]
Former-commit-id: 44861caab97765e8b7121c20c92a40656a69708c
Former-commit-id: 0b7ab0f4024c1a69a60326fa363923bbfab19040
</commit_message>
<xml_diff>
--- a/data/HistoricalElections/Sabato_Ratings/2018-2022 Crystal Ball Senate.xlsx
+++ b/data/HistoricalElections/Sabato_Ratings/2018-2022 Crystal Ball Senate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>year</t>
   </si>
@@ -85,10 +85,13 @@
     <t>MO</t>
   </si>
   <si>
+    <t>MS*</t>
+  </si>
+  <si>
+    <t>Likely R</t>
+  </si>
+  <si>
     <t>MS</t>
-  </si>
-  <si>
-    <t>Likely R</t>
   </si>
   <si>
     <t>Safe R</t>
@@ -244,12 +247,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -262,16 +271,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -288,13 +297,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -314,6 +323,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -513,17 +523,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -551,10 +561,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -802,12 +812,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1094,7 +1104,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1122,10 +1132,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1631,10 +1641,10 @@
         <v>2018</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s" s="2">
         <v>6</v>
@@ -1646,7 +1656,7 @@
         <v>2018</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>5</v>
@@ -1661,7 +1671,7 @@
         <v>2018</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s" s="2">
         <v>14</v>
@@ -1676,10 +1686,10 @@
         <v>2018</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s" s="2">
         <v>6</v>
@@ -1691,7 +1701,7 @@
         <v>2018</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>22</v>
@@ -1706,7 +1716,7 @@
         <v>2018</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>8</v>
@@ -1721,7 +1731,7 @@
         <v>2018</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>5</v>
@@ -1736,7 +1746,7 @@
         <v>2018</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s" s="2">
         <v>8</v>
@@ -1751,7 +1761,7 @@
         <v>2018</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>22</v>
@@ -1766,7 +1776,7 @@
         <v>2018</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s" s="2">
         <v>8</v>
@@ -1781,7 +1791,7 @@
         <v>2018</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s" s="2">
         <v>14</v>
@@ -1796,7 +1806,7 @@
         <v>2018</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s" s="2">
         <v>14</v>
@@ -1811,10 +1821,10 @@
         <v>2018</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s" s="2">
         <v>6</v>
@@ -1826,7 +1836,7 @@
         <v>2018</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>8</v>
@@ -1841,7 +1851,7 @@
         <v>2018</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>18</v>
@@ -1856,7 +1866,7 @@
         <v>2018</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>8</v>
@@ -1871,7 +1881,7 @@
         <v>2018</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>22</v>
@@ -1886,10 +1896,10 @@
         <v>2018</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s" s="2">
         <v>6</v>
@@ -1901,7 +1911,7 @@
         <v>2020</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s" s="2">
         <v>14</v>
@@ -1916,7 +1926,7 @@
         <v>2020</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s" s="2">
         <v>25</v>
@@ -1931,10 +1941,10 @@
         <v>2020</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s" s="2">
         <v>6</v>
@@ -1946,7 +1956,7 @@
         <v>2020</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s" s="2">
         <v>5</v>
@@ -1961,7 +1971,7 @@
         <v>2020</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s" s="2">
         <v>22</v>
@@ -1991,10 +2001,10 @@
         <v>2020</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D41" t="s" s="2">
         <v>6</v>
@@ -2006,10 +2016,10 @@
         <v>2020</v>
       </c>
       <c r="B42" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="C42" t="s" s="2">
-        <v>50</v>
       </c>
       <c r="D42" t="s" s="2">
         <v>6</v>
@@ -2021,7 +2031,7 @@
         <v>2020</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s" s="2">
         <v>14</v>
@@ -2036,10 +2046,10 @@
         <v>2020</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D44" t="s" s="2">
         <v>6</v>
@@ -2051,7 +2061,7 @@
         <v>2020</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s" s="2">
         <v>8</v>
@@ -2066,7 +2076,7 @@
         <v>2020</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s" s="2">
         <v>14</v>
@@ -2081,7 +2091,7 @@
         <v>2020</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s" s="2">
         <v>25</v>
@@ -2096,10 +2106,10 @@
         <v>2020</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s" s="2">
         <v>6</v>
@@ -2141,7 +2151,7 @@
         <v>2020</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C51" t="s" s="2">
         <v>5</v>
@@ -2171,7 +2181,7 @@
         <v>2020</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s" s="2">
         <v>25</v>
@@ -2186,7 +2196,7 @@
         <v>2020</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C54" t="s" s="2">
         <v>14</v>
@@ -2201,7 +2211,7 @@
         <v>2020</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s" s="2">
         <v>5</v>
@@ -2216,10 +2226,10 @@
         <v>2020</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D56" t="s" s="2">
         <v>6</v>
@@ -2231,7 +2241,7 @@
         <v>2020</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C57" t="s" s="2">
         <v>22</v>
@@ -2246,7 +2256,7 @@
         <v>2020</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C58" t="s" s="2">
         <v>8</v>
@@ -2261,7 +2271,7 @@
         <v>2020</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C59" t="s" s="2">
         <v>22</v>
@@ -2276,10 +2286,10 @@
         <v>2020</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C60" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D60" t="s" s="2">
         <v>6</v>
@@ -2291,7 +2301,7 @@
         <v>2020</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C61" t="s" s="2">
         <v>8</v>
@@ -2306,7 +2316,7 @@
         <v>2020</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C62" t="s" s="2">
         <v>8</v>
@@ -2321,7 +2331,7 @@
         <v>2020</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C63" t="s" s="2">
         <v>14</v>
@@ -2336,10 +2346,10 @@
         <v>2020</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C64" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D64" t="s" s="2">
         <v>6</v>
@@ -2351,10 +2361,10 @@
         <v>2020</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D65" t="s" s="2">
         <v>6</v>
@@ -2366,7 +2376,7 @@
         <v>2020</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C66" t="s" s="2">
         <v>14</v>
@@ -2381,7 +2391,7 @@
         <v>2020</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C67" t="s" s="2">
         <v>8</v>
@@ -2396,10 +2406,10 @@
         <v>2020</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C68" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D68" t="s" s="2">
         <v>6</v>
@@ -2411,10 +2421,10 @@
         <v>2020</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C69" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D69" t="s" s="2">
         <v>6</v>
@@ -2426,10 +2436,10 @@
         <v>2022</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C70" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D70" t="s" s="2">
         <v>6</v>
@@ -2441,10 +2451,10 @@
         <v>2022</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C71" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D71" t="s" s="2">
         <v>6</v>
@@ -2456,10 +2466,10 @@
         <v>2022</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C72" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D72" t="s" s="2">
         <v>6</v>
@@ -2486,7 +2496,7 @@
         <v>2022</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s" s="2">
         <v>8</v>
@@ -2501,7 +2511,7 @@
         <v>2022</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C75" t="s" s="2">
         <v>22</v>
@@ -2546,7 +2556,7 @@
         <v>2022</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C78" t="s" s="2">
         <v>14</v>
@@ -2576,7 +2586,7 @@
         <v>2022</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C80" t="s" s="2">
         <v>25</v>
@@ -2591,10 +2601,10 @@
         <v>2022</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C81" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D81" t="s" s="2">
         <v>6</v>
@@ -2606,7 +2616,7 @@
         <v>2022</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C82" t="s" s="2">
         <v>8</v>
@@ -2624,7 +2634,7 @@
         <v>13</v>
       </c>
       <c r="C83" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D83" t="s" s="2">
         <v>6</v>
@@ -2636,10 +2646,10 @@
         <v>2022</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C84" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D84" t="s" s="2">
         <v>6</v>
@@ -2651,10 +2661,10 @@
         <v>2022</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C85" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D85" t="s" s="2">
         <v>6</v>
@@ -2666,10 +2676,10 @@
         <v>2022</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C86" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D86" t="s" s="2">
         <v>6</v>
@@ -2699,7 +2709,7 @@
         <v>23</v>
       </c>
       <c r="C88" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D88" t="s" s="2">
         <v>6</v>
@@ -2711,7 +2721,7 @@
         <v>2022</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C89" t="s" s="2">
         <v>14</v>
@@ -2726,10 +2736,10 @@
         <v>2022</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C90" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D90" t="s" s="2">
         <v>6</v>
@@ -2741,7 +2751,7 @@
         <v>2022</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C91" t="s" s="2">
         <v>5</v>
@@ -2756,7 +2766,7 @@
         <v>2022</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C92" t="s" s="2">
         <v>5</v>
@@ -2771,7 +2781,7 @@
         <v>2022</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C93" t="s" s="2">
         <v>8</v>
@@ -2786,7 +2796,7 @@
         <v>2022</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C94" t="s" s="2">
         <v>14</v>
@@ -2801,10 +2811,10 @@
         <v>2022</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C95" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D95" t="s" s="2">
         <v>6</v>
@@ -2816,7 +2826,7 @@
         <v>2022</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C96" t="s" s="2">
         <v>8</v>
@@ -2831,7 +2841,7 @@
         <v>2022</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C97" t="s" s="2">
         <v>14</v>
@@ -2846,10 +2856,10 @@
         <v>2022</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C98" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D98" t="s" s="2">
         <v>6</v>
@@ -2861,10 +2871,10 @@
         <v>2022</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C99" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D99" t="s" s="2">
         <v>6</v>
@@ -2876,7 +2886,7 @@
         <v>2022</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C100" t="s" s="2">
         <v>25</v>
@@ -2891,7 +2901,7 @@
         <v>2022</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C101" t="s" s="2">
         <v>8</v>
@@ -2906,7 +2916,7 @@
         <v>2022</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C102" t="s" s="2">
         <v>22</v>
@@ -2921,7 +2931,7 @@
         <v>2022</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C103" t="s" s="2">
         <v>14</v>

</xml_diff>